<commit_message>
Working on PEB suggestions.
</commit_message>
<xml_diff>
--- a/Submissions/8-TheEnergyJournal-Resubmission/Responses to MPC reviewers November 2024.xlsx
+++ b/Submissions/8-TheEnergyJournal-Resubmission/Responses to MPC reviewers November 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2022/Submissions/8-TheEnergyJournal-Resubmission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F53C2A9-055A-0D47-8FCE-C34E18DAAA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F628050-74F8-7E41-B4F1-52E66B104DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22880" yWindow="500" windowWidth="28320" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Referee responses" sheetId="1" r:id="rId1"/>
@@ -68,13 +68,6 @@
   </si>
   <si>
     <t>Engineers may like dots to denote a flow, but economists often use lower case letters, with capitals for stocks.</t>
-  </si>
-  <si>
-    <t>Thanks for this comment. 
-We acknowledge that the overdot notation may be unfamiliar for economists. However, the goal of this paper is to bridge disciplines, and the chosen nomenclature will necessarily have unfamiliar elements to both disciplines. 
-To be clear, there are already many aspects of the nomenclature in these papers that are unusual for engineers [G (usually a flux), I (usually mass moment of inertia), p (usually pressure), Re (usually Reynolds number), S (usually suface area), u (usually internal energy), etc.]. So these papers are equal-opportunity offenders. 
-Furthermore, economists are already inconsistent in their use of uppercase and lowercase characters: u or U for utility, l or L for labor, etc.
-We made no changes in response to this comment.</t>
   </si>
   <si>
     <t>Annuity factors preceding a capital cost would be lower case. Is that convention clearer? It may be more familiar to your readers.</t>
@@ -145,9 +138,6 @@
 in the cost of owning and operating the device (or plus any saving), plus the Compensating Variation for the “price” change of the energy service, which is linked to the two substitution effects you’ve just calculated. Indeed, you show this Compensating Variation in the expenditure diagrams (figures 3 and 6) of Part II.</t>
   </si>
   <si>
-    <t>Thank you for this comment. Indeed, the compensating variation is defined as \dotN^\hat - \dotN^* and in order to make this clearer we have added the following line to the financial analysis of the substitution effect "The difference  \dotN^* - \dotN^\hat is the compensating variation from microeconomic analysis that allows the consumer to reach the pre-price change utility after a price change. It is negative as the energy service prices declines."</t>
-  </si>
-  <si>
     <t>I’m not sure what the convention on discounting in studies looking at energy savings and embodied energy – if you wanted to use your numbers to get a cost per MJ actually saved, it would be essential to discount everything, for consistency. It could also be argued that emissions in the near term are worse than those occurring later, since they will be in the atmosphere for more of the period most relevant to those currently alive. (The counter-argument that the carbon per unit of energy may fall over time is probably too speculative for more than a footnote.) It’s a bit odd to discount decommissioning costs but to ignore the issue for the
 initial purchase of the device.</t>
   </si>
@@ -159,12 +149,6 @@
   <si>
     <t>I don’t think you need the parts of the appendix that prove that
 the annuity factor is one over the device lifetime when the interest rate is zero – that’s a standard result in economics, and entirely intuitive (since the annuity factor combines depreciation and the return on outstanding capital, and a zero interest rate gives no return on capital).</t>
-  </si>
-  <si>
-    <t>Thanks for this comment. Perhaps it is interesting to know how these derivations came about. When the reviewer suggested that we include discount rates for money, searched the literature and found a paper that purported to account for time value of money with an annuity factor. The equation was clearly incorrect. So we had to derive these factors ourselves. Given that other papers in this space have done this calculation incorrectly, we needed to prove these results to ourselves before we introduced our approach in the paper. That's the first reason we believe there is value in including these proofs in an appendix.
-We point out that these papers have two audiences, economists and energy analysts. We agree with the reviewer that economists will expect that the annuity factor tau = 1.0 when interest rate r = 0 %/year. Economists can ignore those sections of the appendix.
-That said, the equations for the tau values may not be obvious to energy analysts. And the proofs demonstrate the expected behavior, assisting with understanding from this other important audience for these papers, energy analysis.
-We made no changes in response to this comment.</t>
   </si>
   <si>
     <t>Thank you for this insightful comment. We agree with the reviewer that in the aggregate, technology adoption usually follows a logistic (or s) curve. To address this comment, we took two steps. 
@@ -359,6 +343,21 @@
   <si>
     <t>Thank you very much for this good comment and exhorting us to be precise about what we are depicting. In response, we deleted the reference to the Buera and Trachter paper and industrial policy and instead focused on the data in the more relevant Foerster et al. paper, which looks squarely at the long-run effects of sectoral output shocks on aggregate output, including specifically of durable goods, from which we derive the value of 3 for our multiplier. We continue to believe that this is a better approach than using Keynesian multipliers as it is faithful to our sector-specific technology shock, rather than starting with aggregate shocks.</t>
   </si>
+  <si>
+    <t>Thanks for this comment. 
+We acknowledge that the overdot notation may be unfamiliar for economists. However, the goal of this paper is to bridge disciplines, and the chosen nomenclature will necessarily have unfamiliar elements to both disciplines. 
+To be clear, there are already many aspects of the nomenclature in these papers that are unusual for engineers [G (usually a flux), I (usually mass moment of inertia), p (usually pressure), Re (usually Reynolds number), S (usually suface area), u (usually internal energy), etc.]. So these papers are equal-opportunity offenders. 
+Furthermore, economists are already inconsistent in their use of uppercase and lowercase characters: u or U for utility, l or L for labor, etc.
+In response to this comment, we added the following sentence to footnote 4: "As the goal of this paper is to bridge disciplines, the nomenclature will necessarily have unfamiliar elements to each discipline involved."</t>
+  </si>
+  <si>
+    <t>Thank you for this comment. Indeed, the compensating variation is defined as N_dot_hat - N_dot_star. To make this clearer we have added the following line to the financial analysis of the substitution effect "The difference N_dot_star - N_dot_hat is the compensating variation from microeconomic analysis that allows the consumer to reach the pre-price change utility after a price change. It is negative as the energy service prices declines."</t>
+  </si>
+  <si>
+    <t>Thanks for this comment. Perhaps it is interesting to know how these derivations came about. When the reviewer suggested that we include discount rates for money, we searched the literature and found a paper that purported to account for time value of money with an annuity factor. The equation was clearly incorrect. So we (economist and energy analysts) had to derive these factors ourselves. Given that other papers in this space have done this calculation incorrectly, we needed to prove our approach to ourselves before we introduced our approach in the paper. Thus, we believe there is value in including these proofs in an appendix.
+Also, we point out that these papers have two audiences, economists and energy analysts. Parts of the paper will seem obvious to energy analysts. Other parts of the paper will be obvious to economists. Our stated goal is to write a paper that bridges disciplines. A way to achieve that goal is to provide derivations and further additional details in appendices for consultation by both energy analysts and economists. Thus, there may be more appendices than typically seen in such papers, but this owes to the need to serve and join two reseach communities.parts of the paper for energy analysts may appear obvious, whislt other parts may be obvious to economists'. One of our goals was to provide an accessible framework that crosses disciplines. Part of that accessiblity goal is met by providing derviations and further additional details in appendices, for consultation by both energy analysts and eocnomists. Thus there may be more appendices than typically seen, but this is owing to the need to serve and join two research communities'. Then you coudl thank the reviewer, by syaing that their point has reinforced the importance of highlight this twin goal, which you added as a note/footnote.parts of the paper for energy analysts may appear obvious, whislt other parts may be obvious to economists'. One of our goals was to provide an accessible framework that crosses disciplines. Part of that accessiblity goal is met by providing derviations and further additional details in appendices, for consultation by both energy analysts and eocnomists. Thus there may be more appendices than typically seen, but this is owing to the need to serve and join two research communities'. Then you coudl thank the reviewer, by syaing that their point has reinforced the importance of highlight this twin goal, which you added as a note/footnote. 
+This point has reinforced the importance of highlighting our objectives. In response, we which you added a new footnote</t>
+  </si>
 </sst>
 </file>
 
@@ -434,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -454,32 +453,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -703,8 +686,8 @@
   <dimension ref="A1:E760"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -737,371 +720,371 @@
       <c r="B2" s="6"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:5" s="10" customFormat="1" ht="116" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7">
+    <row r="3" spans="1:5" ht="116" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="98" x14ac:dyDescent="0.15">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="126" x14ac:dyDescent="0.15">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="210" x14ac:dyDescent="0.15">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="238" x14ac:dyDescent="0.15">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8">
+        <v>7</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8">
+        <v>8</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="56" x14ac:dyDescent="0.15">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="8">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" ht="196" x14ac:dyDescent="0.15">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12" s="8">
+        <v>10</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="84" x14ac:dyDescent="0.15">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13" s="8">
+        <v>11</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="140" x14ac:dyDescent="0.15">
+      <c r="A14" s="6">
+        <v>1</v>
+      </c>
+      <c r="B14" s="8">
+        <v>12</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="10" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A4" s="7">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="140" x14ac:dyDescent="0.15">
+      <c r="A15" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B15" s="8">
+        <v>13</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" ht="397" x14ac:dyDescent="0.15">
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8">
+        <v>14</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="182" x14ac:dyDescent="0.15">
+      <c r="A17" s="6">
+        <v>1</v>
+      </c>
+      <c r="B17" s="8">
+        <v>15</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A18" s="6">
+        <v>1</v>
+      </c>
+      <c r="B18" s="8">
+        <v>16</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="126" x14ac:dyDescent="0.15">
+      <c r="A19" s="6">
+        <v>1</v>
+      </c>
+      <c r="B19" s="8">
+        <v>17</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A20" s="6">
+        <v>1</v>
+      </c>
+      <c r="B20" s="8">
+        <v>18</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="80" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="6">
+        <v>1</v>
+      </c>
+      <c r="B21" s="8">
+        <v>19</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A22" s="1"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" ht="348" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" s="10" customFormat="1" ht="98" x14ac:dyDescent="0.15">
-      <c r="A5" s="7">
-        <v>1</v>
-      </c>
-      <c r="B5" s="11">
-        <v>3</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" s="10" customFormat="1" ht="126" x14ac:dyDescent="0.15">
-      <c r="A6" s="7">
-        <v>1</v>
-      </c>
-      <c r="B6" s="11">
-        <v>4</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" s="10" customFormat="1" ht="210" x14ac:dyDescent="0.15">
-      <c r="A7" s="7">
-        <v>1</v>
-      </c>
-      <c r="B7" s="11">
-        <v>5</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" s="10" customFormat="1" ht="210" x14ac:dyDescent="0.15">
-      <c r="A8" s="7">
-        <v>1</v>
-      </c>
-      <c r="B8" s="11">
-        <v>6</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="1:5" s="10" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A9" s="7">
-        <v>1</v>
-      </c>
-      <c r="B9" s="11">
-        <v>7</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5" s="10" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A10" s="7">
-        <v>1</v>
-      </c>
-      <c r="B10" s="11">
-        <v>8</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" s="10" customFormat="1" ht="56" x14ac:dyDescent="0.15">
-      <c r="A11" s="7">
-        <v>1</v>
-      </c>
-      <c r="B11" s="11">
-        <v>9</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="9" t="s">
+      <c r="B23" s="8">
         <v>20</v>
       </c>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" s="10" customFormat="1" ht="196" x14ac:dyDescent="0.15">
-      <c r="A12" s="7">
-        <v>1</v>
-      </c>
-      <c r="B12" s="11">
-        <v>10</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="C23" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="249" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1">
+        <v>2</v>
+      </c>
+      <c r="B24" s="8">
         <v>21</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="C24" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" ht="126" x14ac:dyDescent="0.15">
+      <c r="A25" s="1">
+        <v>2</v>
+      </c>
+      <c r="B25" s="8">
         <v>22</v>
       </c>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" s="10" customFormat="1" ht="84" x14ac:dyDescent="0.15">
-      <c r="A13" s="7">
-        <v>1</v>
-      </c>
-      <c r="B13" s="11">
-        <v>11</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="C25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="196" x14ac:dyDescent="0.15">
+      <c r="A26" s="1">
+        <v>2</v>
+      </c>
+      <c r="B26" s="8">
         <v>23</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="C26" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="168" x14ac:dyDescent="0.15">
+      <c r="A27" s="1">
+        <v>2</v>
+      </c>
+      <c r="B27" s="8">
         <v>24</v>
       </c>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" s="10" customFormat="1" ht="140" x14ac:dyDescent="0.15">
-      <c r="A14" s="7">
-        <v>1</v>
-      </c>
-      <c r="B14" s="11">
-        <v>12</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" s="10" customFormat="1" ht="140" x14ac:dyDescent="0.15">
-      <c r="A15" s="7">
-        <v>1</v>
-      </c>
-      <c r="B15" s="11">
-        <v>13</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="1:5" s="10" customFormat="1" ht="238" x14ac:dyDescent="0.15">
-      <c r="A16" s="7">
-        <v>1</v>
-      </c>
-      <c r="B16" s="11">
-        <v>14</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:5" s="10" customFormat="1" ht="182" x14ac:dyDescent="0.15">
-      <c r="A17" s="7">
-        <v>1</v>
-      </c>
-      <c r="B17" s="11">
-        <v>15</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" s="10" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A18" s="7">
-        <v>1</v>
-      </c>
-      <c r="B18" s="11">
-        <v>16</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:5" s="10" customFormat="1" ht="126" x14ac:dyDescent="0.15">
-      <c r="A19" s="7">
-        <v>1</v>
-      </c>
-      <c r="B19" s="11">
-        <v>17</v>
-      </c>
-      <c r="C19" s="15" t="s">
+      <c r="C27" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="1:5" s="10" customFormat="1" ht="42" x14ac:dyDescent="0.15">
-      <c r="A20" s="7">
-        <v>1</v>
-      </c>
-      <c r="B20" s="11">
-        <v>18</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="1:5" s="10" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="7">
-        <v>1</v>
-      </c>
-      <c r="B21" s="11">
-        <v>19</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A22" s="14"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="1:5" s="10" customFormat="1" ht="348" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="14">
-        <v>2</v>
-      </c>
-      <c r="B23" s="11">
-        <v>20</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" s="10" customFormat="1" ht="249" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="14">
-        <v>2</v>
-      </c>
-      <c r="B24" s="11">
-        <v>21</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="12"/>
-    </row>
-    <row r="25" spans="1:5" s="10" customFormat="1" ht="126" x14ac:dyDescent="0.15">
-      <c r="A25" s="14">
-        <v>2</v>
-      </c>
-      <c r="B25" s="11">
-        <v>22</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="1:5" s="10" customFormat="1" ht="196" x14ac:dyDescent="0.15">
-      <c r="A26" s="14">
-        <v>2</v>
-      </c>
-      <c r="B26" s="11">
-        <v>23</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="1:5" s="10" customFormat="1" ht="168" x14ac:dyDescent="0.15">
-      <c r="A27" s="14">
-        <v>2</v>
-      </c>
-      <c r="B27" s="11">
-        <v>24</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="12"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>

</xml_diff>